<commit_message>
saved widgets, added conda pip lists
</commit_message>
<xml_diff>
--- a/model1_config_df.xlsx
+++ b/model1_config_df.xlsx
@@ -422,7 +422,7 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>lstm_23</t>
+          <t>lstm_1</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
@@ -813,7 +813,7 @@
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>lstm_24</t>
+          <t>lstm_2</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr">
@@ -1174,7 +1174,7 @@
       </c>
       <c r="B58" s="1" t="inlineStr">
         <is>
-          <t>dense_12</t>
+          <t>dense_1</t>
         </is>
       </c>
       <c r="C58" s="1" t="inlineStr">

</xml_diff>

<commit_message>
working on laptop. check widgets
</commit_message>
<xml_diff>
--- a/model1_config_df.xlsx
+++ b/model1_config_df.xlsx
@@ -422,7 +422,7 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>lstm_1</t>
+          <t>lstm_5</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
@@ -549,7 +549,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>(None, 14, 1)</t>
+          <t>(None, 7, 1)</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>lstm_2</t>
+          <t>lstm_6</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr">
@@ -1174,7 +1174,7 @@
       </c>
       <c r="B58" s="1" t="inlineStr">
         <is>
-          <t>dense_1</t>
+          <t>dense_3</t>
         </is>
       </c>
       <c r="C58" s="1" t="inlineStr">

</xml_diff>

<commit_message>
renamed nb to _JMI_WIP, model 2 ~complete
</commit_message>
<xml_diff>
--- a/model1_config_df.xlsx
+++ b/model1_config_df.xlsx
@@ -379,7 +379,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,7 +422,7 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>lstm_5</t>
+          <t>lstm_1</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
@@ -808,29 +808,25 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>1: LSTM</t>
+          <t>1: Dropout</t>
         </is>
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>lstm_6</t>
+          <t>dropout_1</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr">
         <is>
-          <t>kernel_initializer  (VarianceScaling):</t>
+          <t>top-level</t>
         </is>
       </c>
       <c r="D31" s="1" t="inlineStr">
         <is>
-          <t>distribution</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>uniform</t>
-        </is>
-      </c>
+          <t>noise_shape</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n"/>
@@ -838,13 +834,11 @@
       <c r="C32" s="1" t="n"/>
       <c r="D32" s="1" t="inlineStr">
         <is>
-          <t>mode</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>fan_avg</t>
-        </is>
+          <t>rate</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="33">
@@ -853,12 +847,10 @@
       <c r="C33" s="1" t="n"/>
       <c r="D33" s="1" t="inlineStr">
         <is>
-          <t>scale</t>
-        </is>
-      </c>
-      <c r="E33" t="n">
-        <v>1</v>
-      </c>
+          <t>seed</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n"/>
@@ -866,26 +858,38 @@
       <c r="C34" s="1" t="n"/>
       <c r="D34" s="1" t="inlineStr">
         <is>
-          <t>seed</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr"/>
+          <t>trainable</t>
+        </is>
+      </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n"/>
-      <c r="B35" s="1" t="n"/>
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>2: LSTM</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>lstm_2</t>
+        </is>
+      </c>
       <c r="C35" s="1" t="inlineStr">
         <is>
-          <t>recurrent_initializer  (Orthogonal):</t>
+          <t>kernel_initializer  (VarianceScaling):</t>
         </is>
       </c>
       <c r="D35" s="1" t="inlineStr">
         <is>
-          <t>gain</t>
-        </is>
-      </c>
-      <c r="E35" t="n">
-        <v>1</v>
+          <t>distribution</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -894,28 +898,26 @@
       <c r="C36" s="1" t="n"/>
       <c r="D36" s="1" t="inlineStr">
         <is>
-          <t>seed</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr"/>
+          <t>mode</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>fan_avg</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n"/>
       <c r="B37" s="1" t="n"/>
-      <c r="C37" s="1" t="inlineStr">
-        <is>
-          <t>top-level</t>
-        </is>
-      </c>
+      <c r="C37" s="1" t="n"/>
       <c r="D37" s="1" t="inlineStr">
         <is>
-          <t>activation</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>relu</t>
-        </is>
+          <t>scale</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -924,7 +926,7 @@
       <c r="C38" s="1" t="n"/>
       <c r="D38" s="1" t="inlineStr">
         <is>
-          <t>activity_regularizer</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
@@ -932,13 +934,19 @@
     <row r="39">
       <c r="A39" s="1" t="n"/>
       <c r="B39" s="1" t="n"/>
-      <c r="C39" s="1" t="n"/>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>recurrent_initializer  (Orthogonal):</t>
+        </is>
+      </c>
       <c r="D39" s="1" t="inlineStr">
         <is>
-          <t>bias_constraint</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr"/>
+          <t>gain</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n"/>
@@ -946,7 +954,7 @@
       <c r="C40" s="1" t="n"/>
       <c r="D40" s="1" t="inlineStr">
         <is>
-          <t>bias_regularizer</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
@@ -954,14 +962,20 @@
     <row r="41">
       <c r="A41" s="1" t="n"/>
       <c r="B41" s="1" t="n"/>
-      <c r="C41" s="1" t="n"/>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>top-level</t>
+        </is>
+      </c>
       <c r="D41" s="1" t="inlineStr">
         <is>
-          <t>dropout</t>
-        </is>
-      </c>
-      <c r="E41" t="n">
-        <v>0</v>
+          <t>activation</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>relu</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -970,12 +984,10 @@
       <c r="C42" s="1" t="n"/>
       <c r="D42" s="1" t="inlineStr">
         <is>
-          <t>go_backwards</t>
-        </is>
-      </c>
-      <c r="E42" t="b">
-        <v>0</v>
-      </c>
+          <t>activity_regularizer</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n"/>
@@ -983,12 +995,10 @@
       <c r="C43" s="1" t="n"/>
       <c r="D43" s="1" t="inlineStr">
         <is>
-          <t>implementation</t>
-        </is>
-      </c>
-      <c r="E43" t="n">
-        <v>1</v>
-      </c>
+          <t>bias_constraint</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n"/>
@@ -996,7 +1006,7 @@
       <c r="C44" s="1" t="n"/>
       <c r="D44" s="1" t="inlineStr">
         <is>
-          <t>kernel_constraint</t>
+          <t>bias_regularizer</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
@@ -1007,10 +1017,12 @@
       <c r="C45" s="1" t="n"/>
       <c r="D45" s="1" t="inlineStr">
         <is>
-          <t>kernel_regularizer</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr"/>
+          <t>dropout</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n"/>
@@ -1018,13 +1030,11 @@
       <c r="C46" s="1" t="n"/>
       <c r="D46" s="1" t="inlineStr">
         <is>
-          <t>recurrent_activation</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>hard_sigmoid</t>
-        </is>
+          <t>go_backwards</t>
+        </is>
+      </c>
+      <c r="E46" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1033,10 +1043,12 @@
       <c r="C47" s="1" t="n"/>
       <c r="D47" s="1" t="inlineStr">
         <is>
-          <t>recurrent_constraint</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr"/>
+          <t>implementation</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n"/>
@@ -1044,12 +1056,10 @@
       <c r="C48" s="1" t="n"/>
       <c r="D48" s="1" t="inlineStr">
         <is>
-          <t>recurrent_dropout</t>
-        </is>
-      </c>
-      <c r="E48" t="n">
-        <v>0</v>
-      </c>
+          <t>kernel_constraint</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n"/>
@@ -1057,7 +1067,7 @@
       <c r="C49" s="1" t="n"/>
       <c r="D49" s="1" t="inlineStr">
         <is>
-          <t>recurrent_regularizer</t>
+          <t>kernel_regularizer</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
@@ -1068,11 +1078,13 @@
       <c r="C50" s="1" t="n"/>
       <c r="D50" s="1" t="inlineStr">
         <is>
-          <t>return_sequences</t>
-        </is>
-      </c>
-      <c r="E50" t="b">
-        <v>0</v>
+          <t>recurrent_activation</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>hard_sigmoid</t>
+        </is>
       </c>
     </row>
     <row r="51">
@@ -1081,12 +1093,10 @@
       <c r="C51" s="1" t="n"/>
       <c r="D51" s="1" t="inlineStr">
         <is>
-          <t>return_state</t>
-        </is>
-      </c>
-      <c r="E51" t="b">
-        <v>0</v>
-      </c>
+          <t>recurrent_constraint</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n"/>
@@ -1094,10 +1104,10 @@
       <c r="C52" s="1" t="n"/>
       <c r="D52" s="1" t="inlineStr">
         <is>
-          <t>stateful</t>
-        </is>
-      </c>
-      <c r="E52" t="b">
+          <t>recurrent_dropout</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1107,12 +1117,10 @@
       <c r="C53" s="1" t="n"/>
       <c r="D53" s="1" t="inlineStr">
         <is>
-          <t>trainable</t>
-        </is>
-      </c>
-      <c r="E53" t="b">
-        <v>1</v>
-      </c>
+          <t>recurrent_regularizer</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n"/>
@@ -1120,11 +1128,11 @@
       <c r="C54" s="1" t="n"/>
       <c r="D54" s="1" t="inlineStr">
         <is>
-          <t>unit_forget_bias</t>
+          <t>return_sequences</t>
         </is>
       </c>
       <c r="E54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1133,11 +1141,11 @@
       <c r="C55" s="1" t="n"/>
       <c r="D55" s="1" t="inlineStr">
         <is>
-          <t>units</t>
-        </is>
-      </c>
-      <c r="E55" t="n">
-        <v>50</v>
+          <t>return_state</t>
+        </is>
+      </c>
+      <c r="E55" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1146,7 +1154,7 @@
       <c r="C56" s="1" t="n"/>
       <c r="D56" s="1" t="inlineStr">
         <is>
-          <t>unroll</t>
+          <t>stateful</t>
         </is>
       </c>
       <c r="E56" t="b">
@@ -1159,7 +1167,7 @@
       <c r="C57" s="1" t="n"/>
       <c r="D57" s="1" t="inlineStr">
         <is>
-          <t>use_bias</t>
+          <t>trainable</t>
         </is>
       </c>
       <c r="E57" t="b">
@@ -1167,30 +1175,16 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="inlineStr">
-        <is>
-          <t>2: Dense</t>
-        </is>
-      </c>
-      <c r="B58" s="1" t="inlineStr">
-        <is>
-          <t>dense_3</t>
-        </is>
-      </c>
-      <c r="C58" s="1" t="inlineStr">
-        <is>
-          <t>kernel_initializer  (VarianceScaling):</t>
-        </is>
-      </c>
+      <c r="A58" s="1" t="n"/>
+      <c r="B58" s="1" t="n"/>
+      <c r="C58" s="1" t="n"/>
       <c r="D58" s="1" t="inlineStr">
         <is>
-          <t>distribution</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>uniform</t>
-        </is>
+          <t>unit_forget_bias</t>
+        </is>
+      </c>
+      <c r="E58" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -1199,13 +1193,11 @@
       <c r="C59" s="1" t="n"/>
       <c r="D59" s="1" t="inlineStr">
         <is>
-          <t>mode</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>fan_avg</t>
-        </is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="60">
@@ -1214,11 +1206,11 @@
       <c r="C60" s="1" t="n"/>
       <c r="D60" s="1" t="inlineStr">
         <is>
-          <t>scale</t>
-        </is>
-      </c>
-      <c r="E60" t="n">
-        <v>1</v>
+          <t>unroll</t>
+        </is>
+      </c>
+      <c r="E60" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -1227,27 +1219,37 @@
       <c r="C61" s="1" t="n"/>
       <c r="D61" s="1" t="inlineStr">
         <is>
-          <t>seed</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr"/>
+          <t>use_bias</t>
+        </is>
+      </c>
+      <c r="E61" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="n"/>
-      <c r="B62" s="1" t="n"/>
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>3: Dense</t>
+        </is>
+      </c>
+      <c r="B62" s="1" t="inlineStr">
+        <is>
+          <t>dense_1</t>
+        </is>
+      </c>
       <c r="C62" s="1" t="inlineStr">
         <is>
-          <t>top-level</t>
+          <t>kernel_initializer  (VarianceScaling):</t>
         </is>
       </c>
       <c r="D62" s="1" t="inlineStr">
         <is>
-          <t>activation</t>
+          <t>distribution</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>linear</t>
+          <t>uniform</t>
         </is>
       </c>
     </row>
@@ -1257,10 +1259,14 @@
       <c r="C63" s="1" t="n"/>
       <c r="D63" s="1" t="inlineStr">
         <is>
-          <t>activity_regularizer</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr"/>
+          <t>mode</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>fan_avg</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n"/>
@@ -1268,10 +1274,12 @@
       <c r="C64" s="1" t="n"/>
       <c r="D64" s="1" t="inlineStr">
         <is>
-          <t>bias_constraint</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr"/>
+          <t>scale</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n"/>
@@ -1279,7 +1287,7 @@
       <c r="C65" s="1" t="n"/>
       <c r="D65" s="1" t="inlineStr">
         <is>
-          <t>bias_regularizer</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="E65" t="inlineStr"/>
@@ -1287,13 +1295,21 @@
     <row r="66">
       <c r="A66" s="1" t="n"/>
       <c r="B66" s="1" t="n"/>
-      <c r="C66" s="1" t="n"/>
+      <c r="C66" s="1" t="inlineStr">
+        <is>
+          <t>top-level</t>
+        </is>
+      </c>
       <c r="D66" s="1" t="inlineStr">
         <is>
-          <t>kernel_constraint</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr"/>
+          <t>activation</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n"/>
@@ -1301,7 +1317,7 @@
       <c r="C67" s="1" t="n"/>
       <c r="D67" s="1" t="inlineStr">
         <is>
-          <t>kernel_regularizer</t>
+          <t>activity_regularizer</t>
         </is>
       </c>
       <c r="E67" t="inlineStr"/>
@@ -1312,12 +1328,10 @@
       <c r="C68" s="1" t="n"/>
       <c r="D68" s="1" t="inlineStr">
         <is>
-          <t>trainable</t>
-        </is>
-      </c>
-      <c r="E68" t="b">
-        <v>1</v>
-      </c>
+          <t>bias_constraint</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n"/>
@@ -1325,12 +1339,10 @@
       <c r="C69" s="1" t="n"/>
       <c r="D69" s="1" t="inlineStr">
         <is>
-          <t>units</t>
-        </is>
-      </c>
-      <c r="E69" t="n">
-        <v>1</v>
-      </c>
+          <t>bias_regularizer</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n"/>
@@ -1338,29 +1350,80 @@
       <c r="C70" s="1" t="n"/>
       <c r="D70" s="1" t="inlineStr">
         <is>
+          <t>kernel_constraint</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n"/>
+      <c r="B71" s="1" t="n"/>
+      <c r="C71" s="1" t="n"/>
+      <c r="D71" s="1" t="inlineStr">
+        <is>
+          <t>kernel_regularizer</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n"/>
+      <c r="B72" s="1" t="n"/>
+      <c r="C72" s="1" t="n"/>
+      <c r="D72" s="1" t="inlineStr">
+        <is>
+          <t>trainable</t>
+        </is>
+      </c>
+      <c r="E72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n"/>
+      <c r="B73" s="1" t="n"/>
+      <c r="C73" s="1" t="n"/>
+      <c r="D73" s="1" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n"/>
+      <c r="B74" s="1" t="n"/>
+      <c r="C74" s="1" t="n"/>
+      <c r="D74" s="1" t="inlineStr">
+        <is>
           <t>use_bias</t>
         </is>
       </c>
-      <c r="E70" t="b">
+      <c r="E74" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="17">
     <mergeCell ref="A2:A30"/>
-    <mergeCell ref="A31:A57"/>
-    <mergeCell ref="A58:A70"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A61"/>
+    <mergeCell ref="A62:A74"/>
     <mergeCell ref="B2:B30"/>
-    <mergeCell ref="B31:B57"/>
-    <mergeCell ref="B58:B70"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B35:B61"/>
+    <mergeCell ref="B62:B74"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="C8:C30"/>
     <mergeCell ref="C31:C34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C57"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="C62:C70"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C61"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="C66:C74"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>